<commit_message>
update of the xlsx files
</commit_message>
<xml_diff>
--- a/workbooks/LiborModel.xlsx
+++ b/workbooks/LiborModel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="controls" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">_xll.ADDIN.PRICING.DATE(TODAY())</f>
-        <v>41749</v>
+        <v>41781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>